<commit_message>
backup log and clear FS when full
</commit_message>
<xml_diff>
--- a/tools/Расчет АС-3.xlsx
+++ b/tools/Расчет АС-3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kosoj/Documents/Arduino/Samovar/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9968E6C8-2ADF-1D4F-9893-CEE7EFFB5A64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481D8A9A-E5D6-A643-AAAC-443BE518D896}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{C9282AA8-605C-344B-8032-FA2B417AED2C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" activeTab="1" xr2:uid="{C9282AA8-605C-344B-8032-FA2B417AED2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Расчет базовый" sheetId="1" r:id="rId1"/>
@@ -1135,6 +1135,43 @@
       <alignment vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -1203,6 +1240,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
@@ -1215,8 +1276,28 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1227,72 +1308,6 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -1315,21 +1330,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -1349,10 +1349,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1796,82 +1792,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" hidden="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="70"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="81"/>
     </row>
     <row r="2" spans="1:20" hidden="1">
-      <c r="A2" s="71"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="73"/>
+      <c r="A2" s="82"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="84"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" hidden="1">
-      <c r="A3" s="71"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="73"/>
+      <c r="A3" s="82"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="84"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="71"/>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="73"/>
+      <c r="A4" s="82"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="84"/>
       <c r="P4" s="31" t="s">
         <v>1</v>
       </c>
@@ -1881,21 +1877,21 @@
       <c r="T4" s="1"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="73"/>
+      <c r="A5" s="82"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="84"/>
       <c r="P5" s="30" t="s">
         <v>2</v>
       </c>
@@ -1905,21 +1901,21 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A6" s="74"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="76"/>
+      <c r="A6" s="85"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="87"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -1949,31 +1945,31 @@
       <c r="T7" s="1"/>
     </row>
     <row r="8" spans="1:20" ht="17" thickBot="1">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="79"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="90"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="79"/>
+      <c r="F8" s="90"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="77" t="s">
+      <c r="H8" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="79"/>
+      <c r="I8" s="90"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="77" t="s">
+      <c r="K8" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="79"/>
+      <c r="L8" s="90"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="77" t="s">
+      <c r="N8" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="O8" s="79"/>
+      <c r="O8" s="90"/>
       <c r="P8" s="5" t="s">
         <v>8</v>
       </c>
@@ -2010,18 +2006,18 @@
         <v>0.32000000000000006</v>
       </c>
       <c r="J9" s="2"/>
-      <c r="K9" s="60">
+      <c r="K9" s="71">
         <f>I9+F9</f>
         <v>1.28</v>
       </c>
-      <c r="L9" s="61"/>
+      <c r="L9" s="72"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="62">
+      <c r="N9" s="73">
         <f>C9-K9</f>
         <v>5.12</v>
       </c>
-      <c r="O9" s="63"/>
-      <c r="P9" s="66">
+      <c r="O9" s="74"/>
+      <c r="P9" s="77">
         <f>A9-K9-N9</f>
         <v>9.6000000000000014</v>
       </c>
@@ -2044,9 +2040,9 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="65"/>
-      <c r="P10" s="67"/>
+      <c r="N10" s="75"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="78"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -3097,8 +3093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C5AEE6-2B79-C248-89D2-07DF9BE2110D}">
   <dimension ref="A2:X38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3131,33 +3127,33 @@
   <sheetData>
     <row r="2" spans="1:24" ht="17" thickBot="1"/>
     <row r="3" spans="1:24" ht="17" thickBot="1">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="95" t="s">
+      <c r="B3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="97"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="95" t="s">
+      <c r="F3" s="94"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="97"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="99" t="s">
+      <c r="I3" s="94"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="98"/>
-      <c r="M3" s="99" t="s">
+      <c r="L3" s="61"/>
+      <c r="M3" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="100" t="s">
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="63" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3198,17 +3194,17 @@
         <f>C4-K4</f>
         <v>3.8250000000000002</v>
       </c>
-      <c r="Q4" s="94">
+      <c r="Q4" s="60">
         <f>(A4-K4-M4)</f>
         <v>5.4999999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="26" customHeight="1" thickBot="1">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
     </row>
     <row r="6" spans="1:24" ht="29" thickBot="1">
       <c r="B6" s="28">
@@ -3280,78 +3276,78 @@
       <c r="P9" s="38"/>
     </row>
     <row r="10" spans="1:24" ht="17" customHeight="1">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="84"/>
-      <c r="E10" s="86" t="s">
+      <c r="D10" s="106"/>
+      <c r="E10" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="90" t="s">
+      <c r="F10" s="100" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="59"/>
-      <c r="I10" s="88" t="s">
+      <c r="I10" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="84" t="s">
+      <c r="J10" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="84" t="s">
+      <c r="K10" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="84"/>
-      <c r="M10" s="86" t="s">
+      <c r="L10" s="106"/>
+      <c r="M10" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="90" t="s">
+      <c r="N10" s="100" t="s">
         <v>20</v>
       </c>
       <c r="O10" s="41"/>
-      <c r="Q10" s="88" t="s">
+      <c r="Q10" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="R10" s="84" t="s">
+      <c r="R10" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="S10" s="84" t="s">
+      <c r="S10" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="T10" s="84"/>
-      <c r="U10" s="86" t="s">
+      <c r="T10" s="106"/>
+      <c r="U10" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="V10" s="90" t="s">
+      <c r="V10" s="100" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="89"/>
-      <c r="B11" s="85"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="91"/>
+      <c r="A11" s="96"/>
+      <c r="B11" s="107"/>
+      <c r="C11" s="107"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="101"/>
       <c r="G11" s="59"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="85"/>
-      <c r="L11" s="85"/>
-      <c r="M11" s="87"/>
-      <c r="N11" s="91"/>
+      <c r="I11" s="96"/>
+      <c r="J11" s="107"/>
+      <c r="K11" s="107"/>
+      <c r="L11" s="107"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="101"/>
       <c r="O11" s="41"/>
-      <c r="Q11" s="89"/>
-      <c r="R11" s="85"/>
-      <c r="S11" s="85"/>
-      <c r="T11" s="85"/>
-      <c r="U11" s="87"/>
-      <c r="V11" s="91"/>
+      <c r="Q11" s="96"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="103"/>
+      <c r="V11" s="101"/>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" s="42">
@@ -3377,8 +3373,8 @@
         <f t="shared" ref="G12:G21" si="0">TRUNC(H12)&amp; ":"&amp;TRUNC((H12 - TRUNC(H12)) * 60)</f>
         <v>2:44</v>
       </c>
-      <c r="H12" s="101">
-        <f>E12/B12</f>
+      <c r="H12" s="64">
+        <f t="shared" ref="H12:H22" si="1">E12/B12</f>
         <v>2.7355623100303954</v>
       </c>
       <c r="I12" s="42">
@@ -3398,14 +3394,14 @@
         <v>0.11968085106382979</v>
       </c>
       <c r="N12" s="46">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O12" s="58" t="str">
-        <f t="shared" ref="O12:O21" si="1">TRUNC(P12)&amp; ":"&amp;TRUNC((P12 - TRUNC(P12)) * 60)</f>
+        <f t="shared" ref="O12:O21" si="2">TRUNC(P12)&amp; ":"&amp;TRUNC((P12 - TRUNC(P12)) * 60)</f>
         <v>1:42</v>
       </c>
-      <c r="P12" s="101">
-        <f>M12/J12</f>
+      <c r="P12" s="64">
+        <f t="shared" ref="P12:P22" si="3">M12/J12</f>
         <v>1.709726443768997</v>
       </c>
       <c r="Q12" s="42">
@@ -3425,14 +3421,14 @@
         <v>0.14361702127659576</v>
       </c>
       <c r="V12" s="46">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="W12" s="58" t="str">
-        <f t="shared" ref="W12:W22" si="2">TRUNC(X12)&amp; ":"&amp;TRUNC((X12 - TRUNC(X12)) * 60)</f>
+        <f t="shared" ref="W12:W22" si="4">TRUNC(X12)&amp; ":"&amp;TRUNC((X12 - TRUNC(X12)) * 60)</f>
         <v>2:3</v>
       </c>
-      <c r="X12" s="101">
-        <f>U12/R12</f>
+      <c r="X12" s="64">
+        <f t="shared" ref="X12:X23" si="5">U12/R12</f>
         <v>2.0516717325227964</v>
       </c>
     </row>
@@ -3450,7 +3446,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="45">
-        <f t="shared" ref="E13:E16" si="3">$F$6*C13</f>
+        <f t="shared" ref="E13:E16" si="6">$F$6*C13</f>
         <v>9.5744680851063843E-2</v>
       </c>
       <c r="F13" s="46">
@@ -3460,8 +3456,8 @@
         <f t="shared" si="0"/>
         <v>0:57</v>
       </c>
-      <c r="H13" s="101">
-        <f>E13/B13</f>
+      <c r="H13" s="64">
+        <f t="shared" si="1"/>
         <v>0.95744680851063835</v>
       </c>
       <c r="I13" s="42">
@@ -3477,18 +3473,18 @@
         <v>17</v>
       </c>
       <c r="M13" s="45">
-        <f t="shared" ref="M13" si="4">$F$6*K13</f>
+        <f t="shared" ref="M13" si="7">$F$6*K13</f>
         <v>7.1808510638297879E-2</v>
       </c>
       <c r="N13" s="46">
         <v>0</v>
       </c>
       <c r="O13" s="58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0:30</v>
       </c>
-      <c r="P13" s="101">
-        <f>M13/J13</f>
+      <c r="P13" s="64">
+        <f t="shared" si="3"/>
         <v>0.51291793313069911</v>
       </c>
       <c r="Q13" s="42">
@@ -3504,18 +3500,18 @@
         <v>17</v>
       </c>
       <c r="U13" s="45">
-        <f t="shared" ref="U13" si="5">$F$6*S13</f>
+        <f t="shared" ref="U13" si="8">$F$6*S13</f>
         <v>9.5744680851063843E-2</v>
       </c>
       <c r="V13" s="46">
         <v>0</v>
       </c>
       <c r="W13" s="58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0:41</v>
       </c>
-      <c r="X13" s="101">
-        <f>U13/R13</f>
+      <c r="X13" s="64">
+        <f t="shared" si="5"/>
         <v>0.68389057750759885</v>
       </c>
     </row>
@@ -3533,7 +3529,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9.5744680851063843E-2</v>
       </c>
       <c r="F14" s="46">
@@ -3543,8 +3539,8 @@
         <f t="shared" si="0"/>
         <v>0:28</v>
       </c>
-      <c r="H14" s="101">
-        <f>E14/B14</f>
+      <c r="H14" s="64">
+        <f t="shared" si="1"/>
         <v>0.47872340425531917</v>
       </c>
       <c r="I14" s="42">
@@ -3567,11 +3563,11 @@
         <v>0</v>
       </c>
       <c r="O14" s="58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0:19</v>
       </c>
-      <c r="P14" s="101">
-        <f>M14/J14</f>
+      <c r="P14" s="64">
+        <f t="shared" si="3"/>
         <v>0.31914893617021284</v>
       </c>
       <c r="Q14" s="42">
@@ -3587,18 +3583,18 @@
         <v>17</v>
       </c>
       <c r="U14" s="45">
-        <f t="shared" ref="U14:U16" si="6">$F$6*S14</f>
+        <f t="shared" ref="U14:U16" si="9">$F$6*S14</f>
         <v>9.5744680851063843E-2</v>
       </c>
       <c r="V14" s="46">
         <v>0</v>
       </c>
       <c r="W14" s="58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0:28</v>
       </c>
-      <c r="X14" s="101">
-        <f>U14/R14</f>
+      <c r="X14" s="64">
+        <f t="shared" si="5"/>
         <v>0.47872340425531917</v>
       </c>
     </row>
@@ -3616,7 +3612,7 @@
         <v>17</v>
       </c>
       <c r="E15" s="45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.7872340425531922E-2</v>
       </c>
       <c r="F15" s="46">
@@ -3626,8 +3622,8 @@
         <f t="shared" si="0"/>
         <v>0:9</v>
       </c>
-      <c r="H15" s="101">
-        <f>E15/B15</f>
+      <c r="H15" s="64">
+        <f t="shared" si="1"/>
         <v>0.15957446808510642</v>
       </c>
       <c r="I15" s="42">
@@ -3650,11 +3646,11 @@
         <v>0</v>
       </c>
       <c r="O15" s="58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0:14</v>
       </c>
-      <c r="P15" s="101">
-        <f>M15/J15</f>
+      <c r="P15" s="64">
+        <f t="shared" si="3"/>
         <v>0.23936170212765959</v>
       </c>
       <c r="Q15" s="42">
@@ -3670,18 +3666,18 @@
         <v>17</v>
       </c>
       <c r="U15" s="45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9.5744680851063843E-2</v>
       </c>
       <c r="V15" s="46">
         <v>0</v>
       </c>
       <c r="W15" s="58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0:19</v>
       </c>
-      <c r="X15" s="101">
-        <f>U15/R15</f>
+      <c r="X15" s="64">
+        <f t="shared" si="5"/>
         <v>0.31914893617021284</v>
       </c>
     </row>
@@ -3699,7 +3695,7 @@
         <v>17</v>
       </c>
       <c r="E16" s="45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.7872340425531922E-2</v>
       </c>
       <c r="F16" s="46">
@@ -3709,8 +3705,8 @@
         <f t="shared" si="0"/>
         <v>0:7</v>
       </c>
-      <c r="H16" s="101">
-        <f>E16/B16</f>
+      <c r="H16" s="64">
+        <f t="shared" si="1"/>
         <v>0.11968085106382979</v>
       </c>
       <c r="I16" s="42">
@@ -3733,11 +3729,11 @@
         <v>100</v>
       </c>
       <c r="O16" s="58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0:14</v>
       </c>
-      <c r="P16" s="101">
-        <f>M16/J16</f>
+      <c r="P16" s="64">
+        <f t="shared" si="3"/>
         <v>0.23936170212765959</v>
       </c>
       <c r="Q16" s="42">
@@ -3753,18 +3749,18 @@
         <v>17</v>
       </c>
       <c r="U16" s="45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4.7872340425531922E-2</v>
       </c>
       <c r="V16" s="46">
         <v>100</v>
       </c>
       <c r="W16" s="58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0:7</v>
       </c>
-      <c r="X16" s="101">
-        <f>U16/R16</f>
+      <c r="X16" s="64">
+        <f t="shared" si="5"/>
         <v>0.11968085106382979</v>
       </c>
     </row>
@@ -3792,8 +3788,8 @@
         <f t="shared" si="0"/>
         <v>0:48</v>
       </c>
-      <c r="H17" s="101">
-        <f>E17/B17</f>
+      <c r="H17" s="64">
+        <f t="shared" si="1"/>
         <v>0.81382978723404276</v>
       </c>
       <c r="I17" s="42">
@@ -3813,14 +3809,14 @@
         <v>1.6276595744680855</v>
       </c>
       <c r="N17" s="46">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="O17" s="58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2:2</v>
       </c>
-      <c r="P17" s="101">
-        <f>M17/J17</f>
+      <c r="P17" s="64">
+        <f t="shared" si="3"/>
         <v>2.0345744680851068</v>
       </c>
       <c r="Q17" s="42">
@@ -3843,11 +3839,11 @@
         <v>120</v>
       </c>
       <c r="W17" s="58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0:40</v>
       </c>
-      <c r="X17" s="101">
-        <f>U17/R17</f>
+      <c r="X17" s="64">
+        <f t="shared" si="5"/>
         <v>0.67819148936170237</v>
       </c>
     </row>
@@ -3865,7 +3861,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="45">
-        <f t="shared" ref="E18:E20" si="7">$M$6*C18</f>
+        <f t="shared" ref="E18:E20" si="10">$M$6*C18</f>
         <v>2.8484042553191493</v>
       </c>
       <c r="F18" s="46">
@@ -3875,8 +3871,8 @@
         <f t="shared" si="0"/>
         <v>3:9</v>
       </c>
-      <c r="H18" s="101">
-        <f>E18/B18</f>
+      <c r="H18" s="64">
+        <f t="shared" si="1"/>
         <v>3.1648936170212769</v>
       </c>
       <c r="I18" s="42">
@@ -3896,14 +3892,14 @@
         <v>1.6276595744680855</v>
       </c>
       <c r="N18" s="46">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="O18" s="58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2:42</v>
       </c>
-      <c r="P18" s="101">
-        <f>M18/J18</f>
+      <c r="P18" s="64">
+        <f t="shared" si="3"/>
         <v>2.7127659574468095</v>
       </c>
       <c r="Q18" s="42">
@@ -3919,18 +3915,18 @@
         <v>18</v>
       </c>
       <c r="U18" s="45">
-        <f t="shared" ref="U18:U19" si="8">$M$6*S18</f>
+        <f t="shared" ref="U18:U19" si="11">$M$6*S18</f>
         <v>1.6276595744680855</v>
       </c>
       <c r="V18" s="46">
         <v>130</v>
       </c>
       <c r="W18" s="58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2:2</v>
       </c>
-      <c r="X18" s="101">
-        <f>U18/R18</f>
+      <c r="X18" s="64">
+        <f t="shared" si="5"/>
         <v>2.0345744680851068</v>
       </c>
     </row>
@@ -3948,7 +3944,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.40691489361702138</v>
       </c>
       <c r="F19" s="46">
@@ -3958,8 +3954,8 @@
         <f t="shared" si="0"/>
         <v>0:48</v>
       </c>
-      <c r="H19" s="101">
-        <f>E19/B19</f>
+      <c r="H19" s="64">
+        <f t="shared" si="1"/>
         <v>0.81382978723404276</v>
       </c>
       <c r="I19" s="42">
@@ -3982,11 +3978,11 @@
         <v>0</v>
       </c>
       <c r="O19" s="58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1:1</v>
       </c>
-      <c r="P19" s="101">
-        <f>M19/J19</f>
+      <c r="P19" s="64">
+        <f t="shared" si="3"/>
         <v>1.0172872340425534</v>
       </c>
       <c r="Q19" s="42">
@@ -4002,18 +3998,18 @@
         <v>18</v>
       </c>
       <c r="U19" s="45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.0345744680851068</v>
       </c>
       <c r="V19" s="46">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="W19" s="58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3:23</v>
       </c>
-      <c r="X19" s="101">
-        <f>U19/R19</f>
+      <c r="X19" s="64">
+        <f t="shared" si="5"/>
         <v>3.3909574468085113</v>
       </c>
     </row>
@@ -4031,7 +4027,7 @@
         <v>18</v>
       </c>
       <c r="E20" s="45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.40691489361702138</v>
       </c>
       <c r="F20" s="46">
@@ -4041,8 +4037,8 @@
         <f t="shared" si="0"/>
         <v>1:1</v>
       </c>
-      <c r="H20" s="101">
-        <f>E20/B20</f>
+      <c r="H20" s="64">
+        <f t="shared" si="1"/>
         <v>1.0172872340425534</v>
       </c>
       <c r="I20" s="42">
@@ -4065,11 +4061,11 @@
         <v>0</v>
       </c>
       <c r="O20" s="58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1:21</v>
       </c>
-      <c r="P20" s="101">
-        <f>M20/J20</f>
+      <c r="P20" s="64">
+        <f t="shared" si="3"/>
         <v>1.3563829787234047</v>
       </c>
       <c r="Q20" s="42">
@@ -4092,11 +4088,11 @@
         <v>120</v>
       </c>
       <c r="W20" s="58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0:14</v>
       </c>
-      <c r="X20" s="101">
-        <f>U20/R20</f>
+      <c r="X20" s="64">
+        <f t="shared" si="5"/>
         <v>0.23936170212765959</v>
       </c>
     </row>
@@ -4124,8 +4120,8 @@
         <f t="shared" si="0"/>
         <v>0:9</v>
       </c>
-      <c r="H21" s="101">
-        <f>E21/B21</f>
+      <c r="H21" s="64">
+        <f t="shared" si="1"/>
         <v>0.15957446808510642</v>
       </c>
       <c r="I21" s="42">
@@ -4148,11 +4144,11 @@
         <v>0</v>
       </c>
       <c r="O21" s="58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0:14</v>
       </c>
-      <c r="P21" s="101">
-        <f>M21/J21</f>
+      <c r="P21" s="64">
+        <f t="shared" si="3"/>
         <v>0.23936170212765959</v>
       </c>
       <c r="Q21" s="42">
@@ -4175,11 +4171,11 @@
         <v>0</v>
       </c>
       <c r="W21" s="58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0:35</v>
       </c>
-      <c r="X21" s="101">
-        <f>U21/R21</f>
+      <c r="X21" s="64">
+        <f t="shared" si="5"/>
         <v>0.59840425531914898</v>
       </c>
     </row>
@@ -4207,8 +4203,8 @@
         <f>TRUNC(H22)&amp; ":"&amp;TRUNC((H22 - TRUNC(H22)) * 60)</f>
         <v>0:14</v>
       </c>
-      <c r="H22" s="101">
-        <f>E22/B22</f>
+      <c r="H22" s="64">
+        <f t="shared" si="1"/>
         <v>0.23936170212765959</v>
       </c>
       <c r="I22" s="48">
@@ -4234,8 +4230,8 @@
         <f>TRUNC(P22)&amp; ":"&amp;TRUNC((P22 - TRUNC(P22)) * 60)</f>
         <v>0:28</v>
       </c>
-      <c r="P22" s="101">
-        <f>M22/J22</f>
+      <c r="P22" s="64">
+        <f t="shared" si="3"/>
         <v>0.47872340425531917</v>
       </c>
       <c r="Q22" s="42">
@@ -4258,19 +4254,19 @@
         <v>0</v>
       </c>
       <c r="W22" s="58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0:21</v>
       </c>
-      <c r="X22" s="101">
-        <f>U22/R22</f>
+      <c r="X22" s="64">
+        <f t="shared" si="5"/>
         <v>0.35904255319148937</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="17" thickBot="1">
-      <c r="E23" s="93" t="s">
+      <c r="E23" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="93"/>
+      <c r="F23" s="105"/>
       <c r="G23" s="58" t="str">
         <f>TRUNC(H23)&amp; ":"&amp;TRUNC((H23 - TRUNC(H23)) * 60)</f>
         <v>10:39</v>
@@ -4280,10 +4276,10 @@
         <v>10.659764437689972</v>
       </c>
       <c r="K23" s="53"/>
-      <c r="M23" s="93" t="s">
+      <c r="M23" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="N23" s="93"/>
+      <c r="N23" s="105"/>
       <c r="O23" s="58" t="str">
         <f>TRUNC(P23)&amp; ":"&amp;TRUNC((P23 - TRUNC(P23)) * 60)</f>
         <v>10:51</v>
@@ -4292,19 +4288,19 @@
         <f>SUM(P12:P22)</f>
         <v>10.859612462006082</v>
       </c>
-      <c r="Q23" s="109">
+      <c r="Q23" s="66">
         <v>10</v>
       </c>
-      <c r="R23" s="110">
+      <c r="R23" s="67">
         <v>2</v>
       </c>
-      <c r="S23" s="111">
+      <c r="S23" s="68">
         <v>0.5</v>
       </c>
-      <c r="T23" s="112" t="s">
+      <c r="T23" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="U23" s="113">
+      <c r="U23" s="70">
         <f>$I$6*S23</f>
         <v>0.23936170212765959</v>
       </c>
@@ -4315,8 +4311,8 @@
         <f>TRUNC(X23)&amp; ":"&amp;TRUNC((X23 - TRUNC(X23)) * 60)</f>
         <v>0:7</v>
       </c>
-      <c r="X23" s="101">
-        <f>U23/R23</f>
+      <c r="X23" s="64">
+        <f t="shared" si="5"/>
         <v>0.11968085106382979</v>
       </c>
     </row>
@@ -4325,15 +4321,15 @@
       <c r="F24" s="54"/>
       <c r="Q24" s="53"/>
       <c r="R24" s="53"/>
-      <c r="U24" s="93" t="s">
+      <c r="U24" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="V24" s="93"/>
+      <c r="V24" s="105"/>
       <c r="W24" s="58" t="str">
         <f>TRUNC(X25)&amp; ":"&amp;TRUNC((X25 - TRUNC(X25)) * 60)</f>
         <v>11:4</v>
       </c>
-      <c r="X24" s="102"/>
+      <c r="X24" s="65"/>
     </row>
     <row r="25" spans="1:24">
       <c r="E25" s="53"/>
@@ -4346,244 +4342,244 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="B26" s="92" t="s">
+      <c r="B26" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="92"/>
-      <c r="D26" s="92"/>
-      <c r="I26" s="92" t="s">
+      <c r="C26" s="104"/>
+      <c r="D26" s="104"/>
+      <c r="I26" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="92"/>
-      <c r="K26" s="92"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="104"/>
       <c r="S26" s="55"/>
     </row>
     <row r="27" spans="1:24">
-      <c r="B27" s="80" t="str">
+      <c r="B27" s="97" t="str">
         <f>SUBSTITUTE(D12 &amp; ";"&amp;ROUND(E12,3)* 1000&amp; ";"&amp;B12&amp; ";" &amp;A12&amp;";0;"&amp;F12,",",".")</f>
         <v>H;191;0.07;1;0;166</v>
       </c>
-      <c r="C27" s="81"/>
-      <c r="D27" s="82"/>
-      <c r="I27" s="83" t="str">
+      <c r="C27" s="98"/>
+      <c r="D27" s="99"/>
+      <c r="I27" s="91" t="str">
         <f>SUBSTITUTE(L12 &amp; ";"&amp;ROUND(M12,3)* 1000&amp; ";"&amp;J12&amp; ";" &amp;I12&amp;";0;"&amp;N12,",",".")</f>
-        <v>H;120;0.07;1;0;85</v>
-      </c>
-      <c r="J27" s="83"/>
-      <c r="K27" s="83"/>
-      <c r="Q27" s="103" t="s">
+        <v>H;120;0.07;1;0;90</v>
+      </c>
+      <c r="J27" s="91"/>
+      <c r="K27" s="91"/>
+      <c r="Q27" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="R27" s="104"/>
-      <c r="S27" s="105"/>
+      <c r="R27" s="109"/>
+      <c r="S27" s="110"/>
     </row>
     <row r="28" spans="1:24">
-      <c r="B28" s="80" t="str">
-        <f t="shared" ref="B28:B37" si="9">SUBSTITUTE(D13 &amp; ";"&amp;ROUND(E13,3)* 1000&amp; ";"&amp;B13&amp; ";" &amp;A13&amp;";0;"&amp;F13,",",".")</f>
+      <c r="B28" s="97" t="str">
+        <f t="shared" ref="B28:B37" si="12">SUBSTITUTE(D13 &amp; ";"&amp;ROUND(E13,3)* 1000&amp; ";"&amp;B13&amp; ";" &amp;A13&amp;";0;"&amp;F13,",",".")</f>
         <v>H;96;0.1;1;0;0</v>
       </c>
-      <c r="C28" s="81"/>
-      <c r="D28" s="82"/>
-      <c r="I28" s="83" t="str">
-        <f t="shared" ref="I28:I37" si="10">SUBSTITUTE(L13 &amp; ";"&amp;ROUND(M13,3)* 1000&amp; ";"&amp;J13&amp; ";" &amp;I13&amp;";0;"&amp;N13,",",".")</f>
+      <c r="C28" s="98"/>
+      <c r="D28" s="99"/>
+      <c r="I28" s="91" t="str">
+        <f t="shared" ref="I28:I37" si="13">SUBSTITUTE(L13 &amp; ";"&amp;ROUND(M13,3)* 1000&amp; ";"&amp;J13&amp; ";" &amp;I13&amp;";0;"&amp;N13,",",".")</f>
         <v>H;72;0.14;1;0;0</v>
       </c>
-      <c r="J28" s="83"/>
-      <c r="K28" s="83"/>
-      <c r="Q28" s="106" t="str">
-        <f>SUBSTITUTE(T12 &amp; ";"&amp;ROUND(U12,3)* 1000&amp; ";"&amp;R12&amp; ";" &amp;Q12&amp;";0;"&amp;V12,",",".")</f>
-        <v>H;144;0.07;0;0;85</v>
-      </c>
-      <c r="R28" s="107"/>
-      <c r="S28" s="108"/>
+      <c r="J28" s="91"/>
+      <c r="K28" s="91"/>
+      <c r="Q28" s="111" t="str">
+        <f t="shared" ref="Q28:Q37" si="14">SUBSTITUTE(T12 &amp; ";"&amp;ROUND(U12,3)* 1000&amp; ";"&amp;R12&amp; ";" &amp;Q12&amp;";0;"&amp;V12,",",".")</f>
+        <v>H;144;0.07;0;0;90</v>
+      </c>
+      <c r="R28" s="112"/>
+      <c r="S28" s="113"/>
     </row>
     <row r="29" spans="1:24">
-      <c r="B29" s="80" t="str">
-        <f t="shared" si="9"/>
+      <c r="B29" s="97" t="str">
+        <f t="shared" si="12"/>
         <v>H;96;0.2;2;0;0</v>
       </c>
-      <c r="C29" s="81"/>
-      <c r="D29" s="82"/>
-      <c r="I29" s="83" t="str">
-        <f t="shared" si="10"/>
+      <c r="C29" s="98"/>
+      <c r="D29" s="99"/>
+      <c r="I29" s="91" t="str">
+        <f t="shared" si="13"/>
         <v>H;96;0.3;2;0;0</v>
       </c>
-      <c r="J29" s="83"/>
-      <c r="K29" s="83"/>
-      <c r="Q29" s="106" t="str">
-        <f>SUBSTITUTE(T13 &amp; ";"&amp;ROUND(U13,3)* 1000&amp; ";"&amp;R13&amp; ";" &amp;Q13&amp;";0;"&amp;V13,",",".")</f>
+      <c r="J29" s="91"/>
+      <c r="K29" s="91"/>
+      <c r="Q29" s="111" t="str">
+        <f t="shared" si="14"/>
         <v>H;96;0.14;0;0;0</v>
       </c>
-      <c r="R29" s="107"/>
-      <c r="S29" s="108"/>
+      <c r="R29" s="112"/>
+      <c r="S29" s="113"/>
     </row>
     <row r="30" spans="1:24">
-      <c r="B30" s="80" t="str">
-        <f t="shared" si="9"/>
+      <c r="B30" s="97" t="str">
+        <f t="shared" si="12"/>
         <v>H;48;0.3;3;0;0</v>
       </c>
-      <c r="C30" s="81"/>
-      <c r="D30" s="82"/>
-      <c r="I30" s="83" t="str">
-        <f t="shared" si="10"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="99"/>
+      <c r="I30" s="91" t="str">
+        <f t="shared" si="13"/>
         <v>H;96;0.4;3;0;0</v>
       </c>
-      <c r="J30" s="83"/>
-      <c r="K30" s="83"/>
-      <c r="Q30" s="106" t="str">
-        <f>SUBSTITUTE(T14 &amp; ";"&amp;ROUND(U14,3)* 1000&amp; ";"&amp;R14&amp; ";" &amp;Q14&amp;";0;"&amp;V14,",",".")</f>
+      <c r="J30" s="91"/>
+      <c r="K30" s="91"/>
+      <c r="Q30" s="111" t="str">
+        <f t="shared" si="14"/>
         <v>H;96;0.2;1;0;0</v>
       </c>
-      <c r="R30" s="107"/>
-      <c r="S30" s="108"/>
+      <c r="R30" s="112"/>
+      <c r="S30" s="113"/>
     </row>
     <row r="31" spans="1:24">
-      <c r="B31" s="80" t="str">
-        <f t="shared" si="9"/>
+      <c r="B31" s="97" t="str">
+        <f t="shared" si="12"/>
         <v>H;48;0.4;4;0;0</v>
       </c>
-      <c r="C31" s="81"/>
-      <c r="D31" s="82"/>
-      <c r="I31" s="83" t="str">
-        <f t="shared" si="10"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="99"/>
+      <c r="I31" s="91" t="str">
+        <f t="shared" si="13"/>
         <v>H;96;0.4;4;0;100</v>
       </c>
-      <c r="J31" s="83"/>
-      <c r="K31" s="83"/>
-      <c r="Q31" s="106" t="str">
-        <f>SUBSTITUTE(T15 &amp; ";"&amp;ROUND(U15,3)* 1000&amp; ";"&amp;R15&amp; ";" &amp;Q15&amp;";0;"&amp;V15,",",".")</f>
+      <c r="J31" s="91"/>
+      <c r="K31" s="91"/>
+      <c r="Q31" s="111" t="str">
+        <f t="shared" si="14"/>
         <v>H;96;0.3;2;0;0</v>
       </c>
-      <c r="R31" s="107"/>
-      <c r="S31" s="108"/>
+      <c r="R31" s="112"/>
+      <c r="S31" s="113"/>
     </row>
     <row r="32" spans="1:24">
-      <c r="B32" s="80" t="str">
-        <f t="shared" si="9"/>
+      <c r="B32" s="97" t="str">
+        <f t="shared" si="12"/>
         <v>B;407;0.5;5;0;0</v>
       </c>
-      <c r="C32" s="81"/>
-      <c r="D32" s="82"/>
-      <c r="I32" s="83" t="str">
-        <f t="shared" si="10"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="99"/>
+      <c r="I32" s="91" t="str">
+        <f t="shared" si="13"/>
+        <v>B;1628;0.8;5;0;120</v>
+      </c>
+      <c r="J32" s="91"/>
+      <c r="K32" s="91"/>
+      <c r="Q32" s="111" t="str">
+        <f t="shared" si="14"/>
+        <v>H;48;0.4;3;0;100</v>
+      </c>
+      <c r="R32" s="112"/>
+      <c r="S32" s="113"/>
+    </row>
+    <row r="33" spans="2:19">
+      <c r="B33" s="97" t="str">
+        <f t="shared" si="12"/>
+        <v>B;2848;0.9;6;0;0</v>
+      </c>
+      <c r="C33" s="98"/>
+      <c r="D33" s="99"/>
+      <c r="I33" s="91" t="str">
+        <f t="shared" si="13"/>
+        <v>B;1628;0.6;6;0;150</v>
+      </c>
+      <c r="J33" s="91"/>
+      <c r="K33" s="91"/>
+      <c r="Q33" s="111" t="str">
+        <f t="shared" si="14"/>
+        <v>B;407;0.6;4;0;120</v>
+      </c>
+      <c r="R33" s="112"/>
+      <c r="S33" s="113"/>
+    </row>
+    <row r="34" spans="2:19">
+      <c r="B34" s="97" t="str">
+        <f t="shared" si="12"/>
+        <v>B;407;0.5;7;0;0</v>
+      </c>
+      <c r="C34" s="98"/>
+      <c r="D34" s="99"/>
+      <c r="I34" s="91" t="str">
+        <f t="shared" si="13"/>
+        <v>B;407;0.4;7;0;0</v>
+      </c>
+      <c r="J34" s="91"/>
+      <c r="K34" s="91"/>
+      <c r="Q34" s="111" t="str">
+        <f t="shared" si="14"/>
         <v>B;1628;0.8;5;0;130</v>
       </c>
-      <c r="J32" s="83"/>
-      <c r="K32" s="83"/>
-      <c r="Q32" s="106" t="str">
-        <f>SUBSTITUTE(T16 &amp; ";"&amp;ROUND(U16,3)* 1000&amp; ";"&amp;R16&amp; ";" &amp;Q16&amp;";0;"&amp;V16,",",".")</f>
-        <v>H;48;0.4;3;0;100</v>
-      </c>
-      <c r="R32" s="107"/>
-      <c r="S32" s="108"/>
-    </row>
-    <row r="33" spans="2:19">
-      <c r="B33" s="80" t="str">
-        <f t="shared" si="9"/>
-        <v>B;2848;0.9;6;0;0</v>
-      </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="82"/>
-      <c r="I33" s="83" t="str">
-        <f t="shared" si="10"/>
-        <v>B;1628;0.6;6;0;155</v>
-      </c>
-      <c r="J33" s="83"/>
-      <c r="K33" s="83"/>
-      <c r="Q33" s="106" t="str">
-        <f>SUBSTITUTE(T17 &amp; ";"&amp;ROUND(U17,3)* 1000&amp; ";"&amp;R17&amp; ";" &amp;Q17&amp;";0;"&amp;V17,",",".")</f>
-        <v>B;407;0.6;4;0;120</v>
-      </c>
-      <c r="R33" s="107"/>
-      <c r="S33" s="108"/>
-    </row>
-    <row r="34" spans="2:19">
-      <c r="B34" s="80" t="str">
-        <f t="shared" si="9"/>
-        <v>B;407;0.5;7;0;0</v>
-      </c>
-      <c r="C34" s="81"/>
-      <c r="D34" s="82"/>
-      <c r="I34" s="83" t="str">
-        <f t="shared" si="10"/>
-        <v>B;407;0.4;7;0;0</v>
-      </c>
-      <c r="J34" s="83"/>
-      <c r="K34" s="83"/>
-      <c r="Q34" s="106" t="str">
-        <f>SUBSTITUTE(T18 &amp; ";"&amp;ROUND(U18,3)* 1000&amp; ";"&amp;R18&amp; ";" &amp;Q18&amp;";0;"&amp;V18,",",".")</f>
-        <v>B;1628;0.8;5;0;130</v>
-      </c>
-      <c r="R34" s="107"/>
-      <c r="S34" s="108"/>
+      <c r="R34" s="112"/>
+      <c r="S34" s="113"/>
     </row>
     <row r="35" spans="2:19">
-      <c r="B35" s="80" t="str">
-        <f t="shared" si="9"/>
+      <c r="B35" s="97" t="str">
+        <f t="shared" si="12"/>
         <v>B;407;0.4;8;0;0</v>
       </c>
-      <c r="C35" s="81"/>
-      <c r="D35" s="82"/>
-      <c r="I35" s="83" t="str">
-        <f t="shared" si="10"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="99"/>
+      <c r="I35" s="91" t="str">
+        <f t="shared" si="13"/>
         <v>B;407;0.3;8;0;0</v>
       </c>
-      <c r="J35" s="83"/>
-      <c r="K35" s="83"/>
-      <c r="Q35" s="106" t="str">
-        <f>SUBSTITUTE(T19 &amp; ";"&amp;ROUND(U19,3)* 1000&amp; ";"&amp;R19&amp; ";" &amp;Q19&amp;";0;"&amp;V19,",",".")</f>
-        <v>B;2035;0.6;6;0;155</v>
-      </c>
-      <c r="R35" s="107"/>
-      <c r="S35" s="108"/>
+      <c r="J35" s="91"/>
+      <c r="K35" s="91"/>
+      <c r="Q35" s="111" t="str">
+        <f t="shared" si="14"/>
+        <v>B;2035;0.6;6;0;150</v>
+      </c>
+      <c r="R35" s="112"/>
+      <c r="S35" s="113"/>
     </row>
     <row r="36" spans="2:19">
-      <c r="B36" s="80" t="str">
-        <f t="shared" si="9"/>
+      <c r="B36" s="97" t="str">
+        <f t="shared" si="12"/>
         <v>T;48;0.3;9;0;0</v>
       </c>
-      <c r="C36" s="81"/>
-      <c r="D36" s="82"/>
-      <c r="I36" s="83" t="str">
-        <f t="shared" si="10"/>
+      <c r="C36" s="98"/>
+      <c r="D36" s="99"/>
+      <c r="I36" s="91" t="str">
+        <f t="shared" si="13"/>
         <v>T;48;0.2;9;0;0</v>
       </c>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-      <c r="Q36" s="106" t="str">
-        <f>SUBSTITUTE(T20 &amp; ";"&amp;ROUND(U20,3)* 1000&amp; ";"&amp;R20&amp; ";" &amp;Q20&amp;";0;"&amp;V20,",",".")</f>
+      <c r="J36" s="91"/>
+      <c r="K36" s="91"/>
+      <c r="Q36" s="111" t="str">
+        <f t="shared" si="14"/>
         <v>T;96;0.4;7;0;120</v>
       </c>
-      <c r="R36" s="107"/>
-      <c r="S36" s="108"/>
+      <c r="R36" s="112"/>
+      <c r="S36" s="113"/>
     </row>
     <row r="37" spans="2:19">
-      <c r="B37" s="80" t="str">
-        <f t="shared" si="9"/>
+      <c r="B37" s="97" t="str">
+        <f t="shared" si="12"/>
         <v>T;48;0.2;10;0;0</v>
       </c>
-      <c r="C37" s="81"/>
-      <c r="D37" s="82"/>
-      <c r="I37" s="83" t="str">
-        <f t="shared" si="10"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="99"/>
+      <c r="I37" s="91" t="str">
+        <f t="shared" si="13"/>
         <v>T;48;0.1;10;0;0</v>
       </c>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="Q37" s="106" t="str">
-        <f>SUBSTITUTE(T21 &amp; ";"&amp;ROUND(U21,3)* 1000&amp; ";"&amp;R21&amp; ";" &amp;Q21&amp;";0;"&amp;V21,",",".")</f>
+      <c r="J37" s="91"/>
+      <c r="K37" s="91"/>
+      <c r="Q37" s="111" t="str">
+        <f t="shared" si="14"/>
         <v>T;239;0.4;8;0;0</v>
       </c>
-      <c r="R37" s="107"/>
-      <c r="S37" s="108"/>
+      <c r="R37" s="112"/>
+      <c r="S37" s="113"/>
     </row>
     <row r="38" spans="2:19">
-      <c r="Q38" s="106" t="str">
+      <c r="Q38" s="111" t="str">
         <f>SUBSTITUTE(T23 &amp; ";"&amp;ROUND(U23,3)* 1000&amp; ";"&amp;R23&amp; ";" &amp;Q23&amp;";0;"&amp;V23,",",".")</f>
         <v>T;239;2;10;0;0</v>
       </c>
-      <c r="R38" s="107"/>
-      <c r="S38" s="108"/>
+      <c r="R38" s="112"/>
+      <c r="S38" s="113"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -4599,22 +4595,23 @@
     <mergeCell ref="Q32:S32"/>
     <mergeCell ref="Q33:S33"/>
     <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="K10:L11"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I34:K34"/>
     <mergeCell ref="Q27:S27"/>
     <mergeCell ref="Q28:S28"/>
     <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
     <mergeCell ref="V10:V11"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B28:D28"/>
@@ -4629,16 +4626,8 @@
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="U24:V24"/>
     <mergeCell ref="S10:T11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="K10:L11"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="M23:N23"/>
     <mergeCell ref="I37:K37"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="E3:F3"/>
@@ -4648,6 +4637,13 @@
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B31:D31"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I31:K31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>